<commit_message>
ready for pypi package
</commit_message>
<xml_diff>
--- a/data/test/recepie.xlsx
+++ b/data/test/recepie.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\repos\vodex\data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2FCD2914-5A93-4B4F-8584-057B81474C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970270E6-6A35-47F1-B82F-CED14F4237B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-400" windowWidth="38620" windowHeight="21820" xr2:uid="{E86253B3-A25E-452E-BDAF-12A20302F090}"/>
+    <workbookView xWindow="41390" yWindow="380" windowWidth="15520" windowHeight="19270" xr2:uid="{E86253B3-A25E-452E-BDAF-12A20302F090}"/>
   </bookViews>
   <sheets>
     <sheet name="recepie" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,16 +53,10 @@
     <t>volume</t>
   </si>
   <si>
-    <t>c_stim</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>s_stim</t>
   </si>
   <si>
     <t>light</t>
@@ -80,6 +75,12 @@
   </si>
   <si>
     <t>frame_in_file</t>
+  </si>
+  <si>
+    <t>c_label</t>
+  </si>
+  <si>
+    <t>shape</t>
   </si>
 </sst>
 </file>
@@ -893,7 +894,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -913,22 +914,22 @@
         <v>4</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -947,10 +948,10 @@
         <v>0</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" s="45">
         <v>0</v>
@@ -973,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="44">
         <v>0</v>
@@ -999,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G4" s="44">
         <v>0</v>
@@ -1025,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="44">
         <v>0</v>
@@ -1051,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="44">
         <v>0</v>
@@ -1077,10 +1078,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G7" s="44">
         <v>0</v>
@@ -1103,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="44">
         <v>0</v>
@@ -1129,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="41">
         <v>1</v>
@@ -1155,10 +1156,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="41">
         <v>1</v>
@@ -1181,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G11" s="41">
         <v>1</v>
@@ -1207,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" s="46">
         <v>1</v>
@@ -1235,10 +1236,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G13" s="41">
         <v>1</v>
@@ -1263,10 +1264,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G14" s="41">
         <v>1</v>
@@ -1291,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G15" s="41">
         <v>1</v>
@@ -1319,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G16" s="41">
         <v>1</v>
@@ -1347,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G17" s="41">
         <v>1</v>
@@ -1375,10 +1376,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G18" s="41">
         <v>1</v>
@@ -1403,10 +1404,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G19" s="41">
         <v>1</v>
@@ -1431,10 +1432,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G20" s="41">
         <v>1</v>
@@ -1459,10 +1460,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G21" s="47">
         <v>1</v>
@@ -1487,10 +1488,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G22" s="46">
         <v>1</v>
@@ -1515,10 +1516,10 @@
         <v>2</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G23" s="41">
         <v>1</v>
@@ -1543,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G24" s="41">
         <v>1</v>
@@ -1571,10 +1572,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G25" s="41">
         <v>1</v>
@@ -1599,10 +1600,10 @@
         <v>2</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G26" s="41">
         <v>1</v>
@@ -1627,10 +1628,10 @@
         <v>2</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G27" s="42">
         <v>2</v>
@@ -1655,10 +1656,10 @@
         <v>2</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G28" s="42">
         <v>2</v>
@@ -1683,10 +1684,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G29" s="42">
         <v>2</v>
@@ -1711,10 +1712,10 @@
         <v>2</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G30" s="42">
         <v>2</v>
@@ -1739,10 +1740,10 @@
         <v>2</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G31" s="48">
         <v>2</v>
@@ -1767,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G32" s="42">
         <v>2</v>
@@ -1793,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G33" s="42">
         <v>2</v>
@@ -1819,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G34" s="42">
         <v>2</v>
@@ -1845,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G35" s="42">
         <v>2</v>
@@ -1871,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G36" s="42">
         <v>2</v>
@@ -1897,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G37" s="42">
         <v>2</v>
@@ -1923,10 +1924,10 @@
         <v>0</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G38" s="42">
         <v>2</v>
@@ -1949,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G39" s="42">
         <v>2</v>
@@ -1975,10 +1976,10 @@
         <v>0</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G40" s="42">
         <v>2</v>
@@ -2001,10 +2002,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G41" s="42">
         <v>2</v>
@@ -2027,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G42" s="42">
         <v>2</v>
@@ -2053,10 +2054,10 @@
         <v>1</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G43" s="43">
         <v>2</v>

</xml_diff>